<commit_message>
feat: add half of intro
</commit_message>
<xml_diff>
--- a/structure.xlsx
+++ b/structure.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Диплом\mine\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C0DB04E-1894-458B-9F96-4B3265ED2324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{88BFAA47-E766-4C20-A716-27E115E3DACC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>2. Общая схема и структура Белорусской объединенной энергосистемы.</t>
   </si>
@@ -126,12 +120,15 @@
   <si>
     <t>В интернетах этих</t>
   </si>
+  <si>
+    <t>Общая постановка задачи об оптимизации ДП-1060211521-2020-01-ПЛ.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,16 +212,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -287,7 +284,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -339,7 +336,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -533,27 +530,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF235556-7893-474E-B5EB-6D805FBB558C}">
-  <dimension ref="A1:J18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="79" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -564,205 +561,213 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75">
       <c r="B3">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75">
       <c r="B5">
         <v>3.6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75">
+      <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="D8" s="6" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-      <c r="D9" s="6" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75">
+      <c r="C9" s="6"/>
+      <c r="D9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75">
       <c r="C10">
         <v>55</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75">
       <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75">
+      <c r="D13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C14" s="3"/>
-      <c r="D14" s="2" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75">
+      <c r="C14" s="2"/>
+      <c r="D14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="18" spans="8:8">
       <c r="H18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="D6:J6"/>
     <mergeCell ref="D14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B16:H16"/>
@@ -773,16 +778,11 @@
     <mergeCell ref="D11:J11"/>
     <mergeCell ref="D12:J12"/>
     <mergeCell ref="D13:J13"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="D6:J6"/>
     <mergeCell ref="D7:J7"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="http://energo.by/content/deyatelnost-obedineniya/osnovnye-pokazateli/" xr:uid="{47A1CE1D-7CCF-40BC-B326-051232EDD3FA}"/>
+    <hyperlink ref="A4" r:id="rId1" display="http://energo.by/content/deyatelnost-obedineniya/osnovnye-pokazateli/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
feat: add 1,2 parts
</commit_message>
<xml_diff>
--- a/structure.xlsx
+++ b/structure.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Диплом\fuckingDiplom\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3C878C-A9EB-499C-94D6-66BBC6A443A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="таб1.1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>2. Общая схема и структура Белорусской объединенной энергосистемы.</t>
   </si>
@@ -57,9 +58,6 @@
     <t>Список литературы.</t>
   </si>
   <si>
-    <t xml:space="preserve">Введение </t>
-  </si>
-  <si>
     <t>PDF</t>
   </si>
   <si>
@@ -70,22 +68,6 @@
   </si>
   <si>
     <t>20-25</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Анализ литературы и </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color theme="5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>постановка задачи.</t>
-    </r>
   </si>
   <si>
     <t>Общая схема и структура</t>
@@ -123,12 +105,166 @@
   <si>
     <t>Общая постановка задачи об оптимизации ДП-1060211521-2020-01-ПЛ.</t>
   </si>
+  <si>
+    <t>Введение и постановка задачи</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Анализ литературы и </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>постановка вопросов проекта.</t>
+    </r>
+  </si>
+  <si>
+    <t>Общая схема и структура Белорусской объединенной энергосистемы ДП-1060211521-2020-02-ПЛ.</t>
+  </si>
+  <si>
+    <t>ОСНОВНЫЕ ПОКАЗАТЕЛИ ГПО «БЕЛЭНЕРГО»</t>
+  </si>
+  <si>
+    <t>Установленная мощность на 01.01.2020</t>
+  </si>
+  <si>
+    <t>МВт</t>
+  </si>
+  <si>
+    <t>Выработка электроэнергии источниками ГПО  «Белэнерго»</t>
+  </si>
+  <si>
+    <t>млрд кВтч</t>
+  </si>
+  <si>
+    <t>Отпуск тепловой энергии</t>
+  </si>
+  <si>
+    <t>млн Гкал</t>
+  </si>
+  <si>
+    <t>Экспорт электроэнергии</t>
+  </si>
+  <si>
+    <t>Выработка электроэнергии блок-станциями</t>
+  </si>
+  <si>
+    <t>Потребление электроэнергии в республике</t>
+  </si>
+  <si>
+    <t>Удельные расходы топлива:</t>
+  </si>
+  <si>
+    <t>на отпуск электроэнергии</t>
+  </si>
+  <si>
+    <t>г/кВтч</t>
+  </si>
+  <si>
+    <t>на отпуск тепла</t>
+  </si>
+  <si>
+    <t>кг/Гкал</t>
+  </si>
+  <si>
+    <t>Технологический расход энергии на ее транспорт:</t>
+  </si>
+  <si>
+    <t>в электрических сетях</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>в тепловых сетях</t>
+  </si>
+  <si>
+    <t>Протяженность линий электропередачи на 01.01.2020</t>
+  </si>
+  <si>
+    <t>Всего</t>
+  </si>
+  <si>
+    <t>тыс. км</t>
+  </si>
+  <si>
+    <t>Воздушные ЛЭП напряжением 35-750 кВ, в том числе:  </t>
+  </si>
+  <si>
+    <t>ЛЭП 220–750 кВ</t>
+  </si>
+  <si>
+    <t>ЛЭП 110 кВ</t>
+  </si>
+  <si>
+    <t>ЛЭП 35 кВ</t>
+  </si>
+  <si>
+    <t>Воздушные ЛЭП напряжением 0,4-10 кВ</t>
+  </si>
+  <si>
+    <t>Кабельные линии  электропередачи</t>
+  </si>
+  <si>
+    <t>Протяженность тепловых сетей в однотрубном исчислении</t>
+  </si>
+  <si>
+    <t>7,506  </t>
+  </si>
+  <si>
+    <t>Количество трансформаторных подстанций  35-750 кВ/Количество трансформаторов</t>
+  </si>
+  <si>
+    <t>1 357/2 398</t>
+  </si>
+  <si>
+    <t>ед.</t>
+  </si>
+  <si>
+    <t>ПС 750 кВ</t>
+  </si>
+  <si>
+    <t>ПС 330 кВ</t>
+  </si>
+  <si>
+    <t>34/93</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ</t>
+  </si>
+  <si>
+    <t>ПС 110 кВ</t>
+  </si>
+  <si>
+    <t>732/1 296</t>
+  </si>
+  <si>
+    <t>ПС 35 кВ</t>
+  </si>
+  <si>
+    <t>580/960</t>
+  </si>
+  <si>
+    <t>Количество трансформаторных подстанций ТП 6-10/0,4 кВ</t>
+  </si>
+  <si>
+    <t>Среднесписочная численность персонала</t>
+  </si>
+  <si>
+    <t>тыс. чел.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,8 +312,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,8 +334,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -199,12 +355,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,6 +451,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -530,43 +783,43 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="D5" sqref="D5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="79" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75">
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -575,15 +828,15 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -592,12 +845,12 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>0</v>
@@ -608,8 +861,11 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75">
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3.6</v>
       </c>
@@ -623,9 +879,9 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>2</v>
@@ -637,9 +893,9 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>3</v>
@@ -651,7 +907,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="6"/>
       <c r="D8" s="7" t="s">
         <v>4</v>
@@ -663,7 +919,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75">
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C9" s="6"/>
       <c r="D9" s="7" t="s">
         <v>5</v>
@@ -675,7 +931,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75">
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>55</v>
       </c>
@@ -689,9 +945,9 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75">
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>7</v>
@@ -703,12 +959,12 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75">
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -717,7 +973,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75">
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D13" s="5" t="s">
         <v>8</v>
       </c>
@@ -728,7 +984,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75">
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" s="5" t="s">
         <v>9</v>
@@ -740,7 +996,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75">
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -749,7 +1005,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75">
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -758,16 +1014,11 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="18" spans="8:8">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="D6:J6"/>
     <mergeCell ref="D14:J14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B16:H16"/>
@@ -779,12 +1030,366 @@
     <mergeCell ref="D12:J12"/>
     <mergeCell ref="D13:J13"/>
     <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="D6:J6"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="http://energo.by/content/deyatelnost-obedineniya/osnovnye-pokazateli/"/>
+    <hyperlink ref="A4" r:id="rId1" display="http://energo.by/content/deyatelnost-obedineniya/osnovnye-pokazateli/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7CC960-8B6C-42A8-A574-C48BD20B7C64}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="13">
+        <v>8947.31</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="14">
+        <v>34.94</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="14">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2.37</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4.32</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="14">
+        <v>37.93</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="14">
+        <v>240.7</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="14">
+        <v>166.65</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="14">
+        <v>7.69</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="14">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="14">
+        <v>279.73</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="14">
+        <v>36.81</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="14">
+        <v>7.68</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="14">
+        <v>17.3</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="14">
+        <v>11.83</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="14">
+        <v>202.22</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="14">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="14">
+        <v>44136</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="14">
+        <v>14154</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="14">
+        <v>74646</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="14">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A11:C11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>